<commit_message>
Made more progress with the buildInvoice.py
see changes in readme 3/8/2024
</commit_message>
<xml_diff>
--- a/2024-02-04_00-29-15_pack-group-1_342d6769-dbe7-43e0-bba3-61cbaeaed180-completed.xlsx
+++ b/2024-02-04_00-29-15_pack-group-1_342d6769-dbe7-43e0-bba3-61cbaeaed180-completed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\barcode-Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C85EF5-FCB3-47ED-B9D9-04B05C010DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC6A0AC-D9FF-4E54-9469-816B50810726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,6 +19,7 @@
     <sheet name="Metadata" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -712,11 +713,17 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -730,12 +737,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1066,10 +1067,10 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1090,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="32"/>
@@ -1105,19 +1106,19 @@
       <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="32"/>
@@ -1128,7 +1129,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="32"/>
@@ -1883,7 +1884,7 @@
       </c>
     </row>
     <row r="20" spans="1:29" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="32"/>
@@ -1897,26 +1898,26 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
       <c r="L20" s="32"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="34"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="39" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="32"/>
@@ -2000,7 +2001,7 @@
       </c>
     </row>
     <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="40" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="32"/>
@@ -2037,7 +2038,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="41" t="s">
         <v>92</v>
       </c>
       <c r="B23" s="32"/>
@@ -2074,7 +2075,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="42" t="s">
         <v>93</v>
       </c>
       <c r="B24" s="32"/>
@@ -2111,7 +2112,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="37" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="32"/>
@@ -2148,7 +2149,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="32"/>
@@ -2162,32 +2163,27 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
       <c r="L26" s="32"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="34"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="34"/>
-      <c r="AB26" s="34"/>
-      <c r="AC26" s="34"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="38"/>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
     </row>
   </sheetData>
   <sheetProtection password="DFB5" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="12">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="A4:L4"/>
     <mergeCell ref="A25:L25"/>
     <mergeCell ref="A26:AC26"/>
     <mergeCell ref="A20:AC20"/>
@@ -2195,6 +2191,11 @@
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="A23:L23"/>
     <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="A4:L4"/>
   </mergeCells>
   <conditionalFormatting sqref="K6:K19">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>